<commit_message>
add origin branch delete order to GitOrderPersonSummarize.xlsx
</commit_message>
<xml_diff>
--- a/GitOrderPersonSummarize.xlsx
+++ b/GitOrderPersonSummarize.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Git概述" sheetId="2" r:id="rId1"/>
-    <sheet name="Git常用命令速查表" sheetId="1" r:id="rId2"/>
+    <sheet name="Git" sheetId="3" r:id="rId1"/>
+    <sheet name="Git概述" sheetId="2" r:id="rId2"/>
+    <sheet name="Git常用命令速查表" sheetId="1" r:id="rId3"/>
+    <sheet name="Linux命令速查表" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="181">
   <si>
     <t>git status</t>
   </si>
@@ -211,13 +213,7 @@
     <t>git log</t>
   </si>
   <si>
-    <t>查看所有提交过的版本信息</t>
-  </si>
-  <si>
     <t>git log --oneline</t>
-  </si>
-  <si>
-    <t>简化显示，显示版本号和提交时的备注信息</t>
   </si>
   <si>
     <t>查看"某人"提交记录</t>
@@ -459,13 +455,817 @@
   <si>
     <t>开发方式</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git push --set-upstream origin b_x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git log --prtty=format:"%ci %cn %s"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简化显示：提交日期、提交者、提交日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简化显示，提交版本、提交日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看：所有提交过的版本信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git checkout .</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linux常用命令速查表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件和目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd ..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回上一级目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入个人主目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看当前路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>find xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开文件夹xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收缩当先路径下xxx文件夹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi 文件路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑指定文件（i开始编辑、esc结束编辑、:wq保存并退出）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将工作区内容恢复成本地库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git clean -f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git clean -fd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除当前路径下untracked files，clean之前可通过git clean -nf查看那些</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连目录也一起删掉，clean之前可通过git clean -nfd查看那些将要删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git clean -nf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git clean -nfd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看那些文件将要删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看那些问价和路径将要删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推送新分支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将本地新创建的分支b_x推送至服务端</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git checkout &lt;hash&gt; &lt;filename&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回退指定文件到指定版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git push origin -d yourbranch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除远程分支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除远程分支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解锁：1805099</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前言</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.softwhy.com/article-8651-1.html</t>
+  </si>
+  <si>
+    <t>Git分支新建与合并</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git-scm.com/book/zh/v2/Git-分支-分支的新建与合并</t>
+  </si>
+  <si>
+    <t>使用Git辅助开发肯定要有一套流程标准，否则每一个人的commit提交习惯不同，可能最终会出现比较混乱的局面。
+2010年，有组织制定一套Git开发流程标准，希望大家遵守。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一.分支种类：</t>
+  </si>
+  <si>
+    <t>当在实际应用开发中，特别是比较复杂的项目，Git不可能只存在一个分支。
+比如主分支存放当前线上稳定版代码，
+还有正在进行测试的非稳定版本分支，
+或者还有正在开发新功能的分支。
+开发建议Git有如下分支（不是影响固定，仅供参考）：
+（1）.master
+（2）.develop
+（3）.hotfix
+（4）.release
+（5）.feature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二.分支种类作用介绍：</t>
+  </si>
+  <si>
+    <t>1.master分支：</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>此分支通常用来存放项目的稳定版本，主要特点如下：
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内容来源主要是分支合并过来，不推荐开发者直接</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>commit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>提交。
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>由于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支可以是稳定版本，可以随时上线，所以通常版本标签都是打在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支各个提交之上。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.develop分支：</t>
+  </si>
+  <si>
+    <r>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开发分支通常和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>feature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>特征分支配合使用，它是所有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>feature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>特征分支的基础。
+当在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>feature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支中测试完新开发的功能后，可以将其合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.hotfix分支：</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>当出现紧急问题，比如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>线上分支出现代码问题，可以在此分支中进行修补，修补之后然后再合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">分支。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>特别说明：在合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>主分支的同事，还要合并一份到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支，否则之后将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>时候，可能会导致修复的问题复现。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.release分支：</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>当</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支开发到自认为足够稳定的状态，将此分支合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>release</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支（在此分支进行上线前的最后测试）。
+最后测试完成后，再合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支。
+合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支是非常好理解的，因为要上线运行。合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是因为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>release</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支后续可能还会发现问题，所以要将与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支同步，以防止以后</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>develop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>再合并到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>release</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分支出现问题。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.feature分支：</t>
+  </si>
+  <si>
+    <t>此分支作用其在介绍develop分支的时候已经涉及，在feature进行新功能的开发，开发完成后再合并到develop。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +1320,47 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -613,10 +1454,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -628,11 +1470,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -640,12 +1483,30 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -667,6 +1528,66 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1" descr="a:3:{s:3:\&quot;pic\&quot;;s:43:\&quot;portal/201808/04/001249htotjm4kb8bacj4s.jpg\&quot;;s:5:\&quot;thumb\&quot;;s:0:\&quot;\&quot;;s:6:\&quot;remote\&quot;;N;}"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1695450" y="3105150"/>
+          <a:ext cx="5210175" cy="2343150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1194,9 +2115,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="6" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="K8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+    </row>
+    <row r="34" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B35" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B36" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+    </row>
+    <row r="37" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B37" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B38" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B39" s="21"/>
+    </row>
+    <row r="40" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B40" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B41" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+    </row>
+    <row r="42" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B43" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B44" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+    </row>
+    <row r="45" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B45" s="21"/>
+    </row>
+    <row r="46" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B46" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B47" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B47:K47"/>
+    <mergeCell ref="B2:I4"/>
+    <mergeCell ref="B7:I18"/>
+    <mergeCell ref="B36:K36"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B44:K44"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="L1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -1206,13 +2447,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
-        <v>122</v>
+      <c r="A1" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1223,12 +2464,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F45"/>
+  <dimension ref="B2:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1243,24 +2484,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="27" x14ac:dyDescent="0.15">
-      <c r="B2" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="10"/>
+      <c r="B2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="E2" s="4" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="3" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
@@ -1273,7 +2517,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
@@ -1295,7 +2539,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>8</v>
@@ -1305,10 +2549,10 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="11"/>
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1324,10 +2568,10 @@
         <v>48</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
@@ -1338,22 +2582,22 @@
         <v>50</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="E11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="E11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
@@ -1363,10 +2607,10 @@
       <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="9"/>
+      <c r="E12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B13" s="4" t="s">
@@ -1376,22 +2620,22 @@
         <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="E14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.15">
@@ -1399,55 +2643,55 @@
         <v>52</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B18" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
@@ -1455,157 +2699,159 @@
         <v>60</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="E20" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" s="12"/>
+      <c r="E21" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B23" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="9"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="11"/>
       <c r="D25" s="3"/>
       <c r="E25" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B26" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="9"/>
+      <c r="E28" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="9"/>
       <c r="D30" s="3"/>
       <c r="E30" s="5" t="s">
         <v>3</v>
@@ -1614,13 +2860,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B31" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>32</v>
-      </c>
+    <row r="31" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B31" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="3"/>
       <c r="E31" s="5" t="s">
         <v>0</v>
@@ -1631,159 +2875,354 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="B34" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="9"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B35" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="3"/>
       <c r="E35" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="5"/>
       <c r="F36" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B37" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="5"/>
       <c r="F37" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B38" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B39" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B41" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B42" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B44" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B45" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="D45" s="3"/>
     </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B46" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B47" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B48" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B49" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B50" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="11"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B51" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B34:C34"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Kzh7GBRT9n9W0s2z1e14G7xjrSvL6okT9cpSNREM5ZS+tKnclYlAYPPrlPyfARHzlVD+pPJ/Xs51IMppYdHLPw==" saltValue="EwmhsUXQrAvR/kBvQuKDjw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="18">
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B25:C25"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="4.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="71.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="B2" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="2:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B4" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="B11" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B24:C24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>